<commit_message>
initialized Excel examples and finished intro
</commit_message>
<xml_diff>
--- a/Excel Inputs/Input 1.xlsx
+++ b/Excel Inputs/Input 1.xlsx
@@ -1,27 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOA Articles\Guerrilla_Automation\Excel Inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8C03C7-73E8-4B4E-A920-9E5C45C8B9A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>A0000</t>
+  </si>
+  <si>
+    <t>A1111</t>
+  </si>
+  <si>
+    <t>A2222</t>
+  </si>
+  <si>
+    <t>A3333</t>
+  </si>
+  <si>
+    <t>A4444</t>
+  </si>
+  <si>
+    <t>A5555</t>
+  </si>
+  <si>
+    <t>A7777</t>
+  </si>
+  <si>
+    <t>A8888</t>
+  </si>
+  <si>
+    <t>A9999</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +107,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +395,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>5228</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>4445</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>9560</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>